<commit_message>
update excel file content
</commit_message>
<xml_diff>
--- a/chains/testing/excel.xlsx
+++ b/chains/testing/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soorria.saruva/repos/content-cdn/chains/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09D62DA6-CF58-9943-A397-67FA55C68D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD8D394-067F-1C4A-B5AA-C72846615830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -47,17 +47,23 @@
   </si>
   <si>
     <t>num,ber</t>
+  </si>
+  <si>
+    <t>7/23/2020</t>
+  </si>
+  <si>
+    <t>456.00</t>
+  </si>
+  <si>
+    <t>7,890</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="#,###"/>
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -69,10 +75,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -104,14 +112,14 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,10 +338,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -342,78 +350,81 @@
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>44035</v>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="6">
         <v>44035.375</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G3" s="7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="7">
         <v>123</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>0.98760000000000003</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
-        <v>456</v>
+      <c r="B6" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
-        <v>7890</v>
+      <c r="B7" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="C7">
         <v>6</v>

</xml_diff>

<commit_message>
update excel file again
</commit_message>
<xml_diff>
--- a/chains/testing/excel.xlsx
+++ b/chains/testing/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soorria.saruva/repos/content-cdn/chains/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD8D394-067F-1C4A-B5AA-C72846615830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A506B755-A725-574D-B0EA-A0D598CAE23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>7,890</t>
+  </si>
+  <si>
+    <t>98.76%</t>
+  </si>
+  <si>
+    <t>$123.00</t>
+  </si>
+  <si>
+    <t>23/7/2020  9:00:00 am</t>
   </si>
 </sst>
 </file>
@@ -109,17 +118,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,7 +348,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -351,13 +358,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -365,7 +372,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C2">
@@ -376,22 +383,20 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
-        <v>44035.375</v>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="G3" s="7">
-        <v>123</v>
-      </c>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
-        <v>123</v>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -401,8 +406,8 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.98760000000000003</v>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -412,7 +417,7 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C6">
@@ -423,7 +428,7 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C7">

</xml_diff>

<commit_message>
update chain testing files
</commit_message>
<xml_diff>
--- a/chains/testing/excel.xlsx
+++ b/chains/testing/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soorria.saruva/repos/content-cdn/chains/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7909F39-9C63-B541-8D58-2B4141100FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBE332F-0773-2241-A9D1-3096055C46A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -65,6 +65,24 @@
   </si>
   <si>
     <t>23/7/2020  9:00:00 am</t>
+  </si>
+  <si>
+    <t>list 1</t>
+  </si>
+  <si>
+    <t>list 2</t>
+  </si>
+  <si>
+    <t>[a,b,c]</t>
+  </si>
+  <si>
+    <t>["c","d","e"]</t>
+  </si>
+  <si>
+    <t>list 3</t>
+  </si>
+  <si>
+    <t>['f', 'g', 'h']</t>
   </si>
 </sst>
 </file>
@@ -345,10 +363,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -435,6 +453,39 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update chain testing files for array parsing (#4)
</commit_message>
<xml_diff>
--- a/chains/testing/excel.xlsx
+++ b/chains/testing/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soorria.saruva/repos/content-cdn/chains/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7909F39-9C63-B541-8D58-2B4141100FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBE332F-0773-2241-A9D1-3096055C46A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -65,6 +65,24 @@
   </si>
   <si>
     <t>23/7/2020  9:00:00 am</t>
+  </si>
+  <si>
+    <t>list 1</t>
+  </si>
+  <si>
+    <t>list 2</t>
+  </si>
+  <si>
+    <t>[a,b,c]</t>
+  </si>
+  <si>
+    <t>["c","d","e"]</t>
+  </si>
+  <si>
+    <t>list 3</t>
+  </si>
+  <si>
+    <t>['f', 'g', 'h']</t>
   </si>
 </sst>
 </file>
@@ -345,10 +363,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -435,6 +453,39 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>